<commit_message>
Fix a typo and generate the translations
</commit_message>
<xml_diff>
--- a/i18n/es.xlsx
+++ b/i18n/es.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\wingspan\wingsearch\i18n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\wingsearch\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A960AB7-AA63-4A60-9F99-00D493A55BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190195EF-6263-4C76-BD74-25AFCB81E1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8535" yWindow="2205" windowWidth="28875" windowHeight="17235" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="28800" windowHeight="15885" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -4073,9 +4073,6 @@
     <t>Experto en humedales</t>
   </si>
   <si>
-    <t>Aves que solo pueden vivir en [weland]</t>
-  </si>
-  <si>
     <t>Cualquier ave que solo tenga el icono de [wetland] y ningún otro icono de hábitat.</t>
   </si>
   <si>
@@ -4233,6 +4230,9 @@
   </si>
   <si>
     <t>Aves que comen [rodent]</t>
+  </si>
+  <si>
+    <t>Aves que solo pueden vivir en [wetland]</t>
   </si>
 </sst>
 </file>
@@ -4476,12 +4476,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K447"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="A1:K447"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
@@ -13052,12 +13052,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
@@ -13106,16 +13106,16 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E2" t="s">
         <v>1377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1378</v>
       </c>
       <c r="G2" t="s">
         <v>1322</v>
       </c>
       <c r="H2" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13129,13 +13129,13 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E3" t="s">
         <v>1380</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>1381</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1382</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -13191,13 +13191,13 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>1358</v>
+      </c>
+      <c r="E7" t="s">
         <v>1359</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>1360</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1361</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13231,16 +13231,16 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E9" t="s">
         <v>1389</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1390</v>
       </c>
       <c r="G9" t="s">
         <v>1322</v>
       </c>
       <c r="H9" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -13276,13 +13276,13 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E12" t="s">
         <v>1374</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>1375</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1376</v>
       </c>
       <c r="G12" t="s">
         <v>1323</v>
@@ -13299,13 +13299,13 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E13" t="s">
         <v>1386</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>1387</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1388</v>
       </c>
       <c r="G13" t="s">
         <v>1329</v>
@@ -13333,10 +13333,10 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
+        <v>1354</v>
+      </c>
+      <c r="E15" t="s">
         <v>1355</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1356</v>
       </c>
       <c r="G15" t="s">
         <v>1323</v>
@@ -13353,16 +13353,16 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E16" t="s">
         <v>1392</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>1393</v>
       </c>
-      <c r="F16" t="s">
-        <v>1394</v>
-      </c>
       <c r="G16" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13422,16 +13422,16 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E19" t="s">
         <v>1383</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1384</v>
       </c>
       <c r="G19" t="s">
         <v>1323</v>
       </c>
       <c r="H19" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13445,13 +13445,13 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E20" t="s">
         <v>1352</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>1353</v>
-      </c>
-      <c r="G20" t="s">
-        <v>1354</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13471,7 +13471,7 @@
         <v>1338</v>
       </c>
       <c r="F21" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="G21" t="s">
         <v>1329</v>
@@ -13488,13 +13488,13 @@
         <v>13</v>
       </c>
       <c r="D22" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E22" t="s">
         <v>1368</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>1369</v>
-      </c>
-      <c r="F22" t="s">
-        <v>1370</v>
       </c>
       <c r="G22" t="s">
         <v>1323</v>
@@ -13531,13 +13531,13 @@
         <v>13</v>
       </c>
       <c r="D24" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E24" t="s">
         <v>1357</v>
       </c>
-      <c r="E24" t="s">
-        <v>1358</v>
-      </c>
       <c r="G24" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13551,16 +13551,16 @@
         <v>13</v>
       </c>
       <c r="D25" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E25" t="s">
         <v>1362</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
+        <v>1353</v>
+      </c>
+      <c r="H25" t="s">
         <v>1363</v>
-      </c>
-      <c r="G25" t="s">
-        <v>1354</v>
-      </c>
-      <c r="H25" t="s">
-        <v>1364</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13574,13 +13574,13 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E26" t="s">
         <v>1365</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>1366</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1367</v>
       </c>
       <c r="G26" t="s">
         <v>1329</v>
@@ -13597,16 +13597,16 @@
         <v>13</v>
       </c>
       <c r="D27" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E27" t="s">
         <v>1346</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>1347</v>
       </c>
-      <c r="F27" t="s">
-        <v>1348</v>
-      </c>
       <c r="G27" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13620,10 +13620,10 @@
         <v>13</v>
       </c>
       <c r="D28" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E28" t="s">
         <v>1395</v>
-      </c>
-      <c r="E28" t="s">
-        <v>1396</v>
       </c>
       <c r="G28" t="s">
         <v>1323</v>
@@ -13640,13 +13640,13 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E29" t="s">
         <v>1371</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>1372</v>
-      </c>
-      <c r="G29" t="s">
-        <v>1373</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13686,13 +13686,13 @@
         <v>1342</v>
       </c>
       <c r="E31" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F31" t="s">
         <v>1343</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>1344</v>
-      </c>
-      <c r="G31" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13712,7 +13712,7 @@
         <v>1328</v>
       </c>
       <c r="F32" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="G32" t="s">
         <v>1329</v>
@@ -13976,7 +13976,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
fixed some birds power text, added spanish version icons
</commit_message>
<xml_diff>
--- a/i18n/es.xlsx
+++ b/i18n/es.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\wingsearch\i18n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\wingspan\wingsearch\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190195EF-6263-4C76-BD74-25AFCB81E1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113274EA-ECA8-4146-BD53-E1F9679A4C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4200" windowWidth="28800" windowHeight="15885" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="1394">
   <si>
     <t>id</t>
   </si>
@@ -3923,9 +3923,6 @@
     <t>Todos los jugadores ponen 1 [egg] en 1 ave [cavity] cualquiera. Puedes poner 1 [egg] en 1 ave [cavity] adicional.</t>
   </si>
   <si>
-    <t>Rova 2 nuevas cartas de bonificación y quédate 1.</t>
-  </si>
-  <si>
     <t>Pon 1 [egg] en cada una de tus aves con un nido [bowl]</t>
   </si>
   <si>
@@ -4130,12 +4127,6 @@
     <t>Fotógrafo</t>
   </si>
   <si>
-    <t>Aves con el icono de fotografo</t>
-  </si>
-  <si>
-    <t>En otras versiones la regla es "Aves con colores en el nombre"</t>
-  </si>
-  <si>
     <t>Constructor de plataformas</t>
   </si>
   <si>
@@ -4175,12 +4166,6 @@
     <t>Anatomista</t>
   </si>
   <si>
-    <t>Aves con el icono de anatomisa</t>
-  </si>
-  <si>
-    <t>En otras versiones la regla es "Aves con partes del cuerpo en el nombre"</t>
-  </si>
-  <si>
     <t>Aficionado de jardín</t>
   </si>
   <si>
@@ -4193,12 +4178,6 @@
     <t>Historiador</t>
   </si>
   <si>
-    <t>Aves con el icono de historiador</t>
-  </si>
-  <si>
-    <t>En otras versiones la regla es "Aves con el nombre de una persona"</t>
-  </si>
-  <si>
     <t>Constructor de cercados</t>
   </si>
   <si>
@@ -4211,12 +4190,6 @@
     <t>Cartógrafo</t>
   </si>
   <si>
-    <t>Aves con el icono de cartógrafo</t>
-  </si>
-  <si>
-    <t>En otras versiones la regla es "Aves que tengan terminos de geografía en el nombre"</t>
-  </si>
-  <si>
     <t>Piscicultor</t>
   </si>
   <si>
@@ -4233,6 +4206,24 @@
   </si>
   <si>
     <t>Aves que solo pueden vivir en [wetland]</t>
+  </si>
+  <si>
+    <t>Cualquier ave con un icono de [rodent]. El ave puede comer también otros tipos de alimento.</t>
+  </si>
+  <si>
+    <t>Aves con el icono [anatomist]</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Aves con el icono [historian]</t>
+  </si>
+  <si>
+    <t>Aves con el icono [cartographer]</t>
+  </si>
+  <si>
+    <t>Aves con el icono [photographer]</t>
   </si>
 </sst>
 </file>
@@ -4476,12 +4467,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K447"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="A1:K447"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
@@ -4564,7 +4555,7 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -4587,7 +4578,7 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -4656,7 +4647,7 @@
         <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -4705,7 +4696,7 @@
         <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -4728,7 +4719,7 @@
         <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
@@ -5262,7 +5253,7 @@
         <v>113</v>
       </c>
       <c r="F34" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="H34" t="s">
         <v>18</v>
@@ -5388,6 +5379,9 @@
       <c r="E39" t="s">
         <v>128</v>
       </c>
+      <c r="F39" t="s">
+        <v>1305</v>
+      </c>
       <c r="H39" t="s">
         <v>18</v>
       </c>
@@ -5507,7 +5501,7 @@
         <v>143</v>
       </c>
       <c r="F44" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="K44" t="s">
         <v>18</v>
@@ -5579,7 +5573,7 @@
         <v>152</v>
       </c>
       <c r="F47" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="J47" t="s">
         <v>18</v>
@@ -5619,7 +5613,7 @@
         <v>158</v>
       </c>
       <c r="F49" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="J49" t="s">
         <v>18</v>
@@ -5688,7 +5682,7 @@
         <v>167</v>
       </c>
       <c r="F52" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="K52" t="s">
         <v>18</v>
@@ -5711,7 +5705,7 @@
         <v>170</v>
       </c>
       <c r="F53" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="K53" t="s">
         <v>18</v>
@@ -5734,7 +5728,7 @@
         <v>173</v>
       </c>
       <c r="F54" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="H54" t="s">
         <v>18</v>
@@ -5840,7 +5834,7 @@
         <v>188</v>
       </c>
       <c r="F59" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="I59" t="s">
         <v>18</v>
@@ -5863,7 +5857,7 @@
         <v>191</v>
       </c>
       <c r="F60" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I60" t="s">
         <v>18</v>
@@ -5932,7 +5926,7 @@
         <v>200</v>
       </c>
       <c r="F63" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="I63" t="s">
         <v>18</v>
@@ -6018,7 +6012,7 @@
         <v>212</v>
       </c>
       <c r="F67" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="H67" t="s">
         <v>18</v>
@@ -6084,7 +6078,7 @@
         <v>221</v>
       </c>
       <c r="F70" t="s">
-        <v>1293</v>
+        <v>1246</v>
       </c>
       <c r="H70" t="s">
         <v>18</v>
@@ -6821,6 +6815,9 @@
       <c r="E106" t="s">
         <v>329</v>
       </c>
+      <c r="F106" t="s">
+        <v>1289</v>
+      </c>
       <c r="I106" t="s">
         <v>18</v>
       </c>
@@ -7552,7 +7549,7 @@
         <v>434</v>
       </c>
       <c r="F141" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="K141" t="s">
         <v>18</v>
@@ -8055,7 +8052,7 @@
         <v>509</v>
       </c>
       <c r="F166" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
@@ -8184,7 +8181,7 @@
         <v>527</v>
       </c>
       <c r="F172" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -8221,7 +8218,7 @@
         <v>533</v>
       </c>
       <c r="F174" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="I174" t="s">
         <v>18</v>
@@ -8247,7 +8244,7 @@
         <v>536</v>
       </c>
       <c r="F175" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="I175" t="s">
         <v>18</v>
@@ -8442,7 +8439,7 @@
         <v>563</v>
       </c>
       <c r="F184" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="K184" t="s">
         <v>18</v>
@@ -8654,7 +8651,7 @@
         <v>593</v>
       </c>
       <c r="F194" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="H194" t="s">
         <v>18</v>
@@ -9233,7 +9230,7 @@
         <v>665</v>
       </c>
       <c r="F218" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
@@ -9253,7 +9250,7 @@
         <v>668</v>
       </c>
       <c r="F219" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
@@ -9636,7 +9633,7 @@
         <v>725</v>
       </c>
       <c r="F238" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
@@ -9702,7 +9699,7 @@
         <v>734</v>
       </c>
       <c r="F241" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="I241" t="s">
         <v>18</v>
@@ -9892,7 +9889,7 @@
         <v>758</v>
       </c>
       <c r="F249" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H249" t="s">
         <v>18</v>
@@ -10055,7 +10052,7 @@
         <v>782</v>
       </c>
       <c r="F257" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="H257" t="s">
         <v>18</v>
@@ -10081,7 +10078,7 @@
         <v>785</v>
       </c>
       <c r="F258" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="H258" t="s">
         <v>18</v>
@@ -13052,12 +13049,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
@@ -13066,7 +13063,7 @@
     <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="82.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -13106,16 +13103,16 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="E2" t="s">
-        <v>1377</v>
+        <v>1389</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1390</v>
       </c>
       <c r="G2" t="s">
-        <v>1322</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1378</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13129,13 +13126,13 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="E3" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="G3" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -13171,13 +13168,13 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E6" t="s">
         <v>1320</v>
       </c>
-      <c r="E6" t="s">
-        <v>1321</v>
-      </c>
       <c r="G6" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13191,13 +13188,13 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E7" t="s">
         <v>1358</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>1359</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13211,13 +13208,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E8" t="s">
         <v>1339</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>1340</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13231,16 +13228,16 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>1388</v>
+        <v>1381</v>
       </c>
       <c r="E9" t="s">
-        <v>1389</v>
+        <v>1392</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1390</v>
       </c>
       <c r="G9" t="s">
-        <v>1322</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1390</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -13276,16 +13273,16 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="E12" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="F12" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="G12" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13299,16 +13296,16 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>1385</v>
+        <v>1378</v>
       </c>
       <c r="E13" t="s">
-        <v>1386</v>
+        <v>1379</v>
       </c>
       <c r="F13" t="s">
-        <v>1387</v>
+        <v>1380</v>
       </c>
       <c r="G13" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -13333,13 +13330,13 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E15" t="s">
         <v>1354</v>
       </c>
-      <c r="E15" t="s">
-        <v>1355</v>
-      </c>
       <c r="G15" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -13353,19 +13350,19 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>1391</v>
+        <v>1382</v>
       </c>
       <c r="E16" t="s">
-        <v>1392</v>
+        <v>1383</v>
       </c>
       <c r="F16" t="s">
-        <v>1393</v>
+        <v>1384</v>
       </c>
       <c r="G16" t="s">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1015</v>
       </c>
@@ -13376,19 +13373,19 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E17" t="s">
         <v>1330</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>1331</v>
       </c>
-      <c r="F17" t="s">
-        <v>1332</v>
-      </c>
       <c r="G17" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1016</v>
       </c>
@@ -13399,19 +13396,19 @@
         <v>13</v>
       </c>
       <c r="D18" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E18" t="s">
         <v>1333</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>1334</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>1335</v>
       </c>
-      <c r="G18" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1017</v>
       </c>
@@ -13422,19 +13419,19 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="E19" t="s">
-        <v>1383</v>
+        <v>1391</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1390</v>
       </c>
       <c r="G19" t="s">
-        <v>1323</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1018</v>
       </c>
@@ -13445,16 +13442,16 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E20" t="s">
         <v>1351</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>1352</v>
       </c>
-      <c r="G20" t="s">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1019</v>
       </c>
@@ -13465,19 +13462,19 @@
         <v>13</v>
       </c>
       <c r="D21" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E21" t="s">
         <v>1337</v>
       </c>
-      <c r="E21" t="s">
-        <v>1338</v>
-      </c>
       <c r="F21" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="G21" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1020</v>
       </c>
@@ -13488,19 +13485,19 @@
         <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="E22" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="F22" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="G22" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1021</v>
       </c>
@@ -13511,16 +13508,16 @@
         <v>13</v>
       </c>
       <c r="D23" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E23" t="s">
         <v>1324</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>1325</v>
       </c>
-      <c r="G23" t="s">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1022</v>
       </c>
@@ -13531,16 +13528,16 @@
         <v>13</v>
       </c>
       <c r="D24" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E24" t="s">
         <v>1356</v>
       </c>
-      <c r="E24" t="s">
-        <v>1357</v>
-      </c>
       <c r="G24" t="s">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1023</v>
       </c>
@@ -13551,19 +13548,19 @@
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E25" t="s">
-        <v>1362</v>
+        <v>1393</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1390</v>
       </c>
       <c r="G25" t="s">
-        <v>1353</v>
-      </c>
-      <c r="H25" t="s">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1024</v>
       </c>
@@ -13574,19 +13571,19 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="E26" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="F26" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="G26" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1025</v>
       </c>
@@ -13597,19 +13594,19 @@
         <v>13</v>
       </c>
       <c r="D27" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E27" t="s">
         <v>1345</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>1346</v>
       </c>
-      <c r="F27" t="s">
-        <v>1347</v>
-      </c>
       <c r="G27" t="s">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1026</v>
       </c>
@@ -13620,16 +13617,19 @@
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>1394</v>
+        <v>1385</v>
       </c>
       <c r="E28" t="s">
-        <v>1395</v>
+        <v>1386</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1388</v>
       </c>
       <c r="G28" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1027</v>
       </c>
@@ -13640,16 +13640,16 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="E29" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="G29" t="s">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1028</v>
       </c>
@@ -13660,19 +13660,19 @@
         <v>13</v>
       </c>
       <c r="D30" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E30" t="s">
         <v>1317</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>1318</v>
       </c>
-      <c r="F30" t="s">
-        <v>1319</v>
-      </c>
       <c r="G30" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1029</v>
       </c>
@@ -13683,19 +13683,19 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F31" t="s">
         <v>1342</v>
       </c>
-      <c r="E31" t="s">
-        <v>1396</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>1343</v>
       </c>
-      <c r="G31" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1030</v>
       </c>
@@ -13706,16 +13706,16 @@
         <v>13</v>
       </c>
       <c r="D32" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E32" t="s">
         <v>1327</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
+        <v>1348</v>
+      </c>
+      <c r="G32" t="s">
         <v>1328</v>
-      </c>
-      <c r="F32" t="s">
-        <v>1349</v>
-      </c>
-      <c r="G32" t="s">
-        <v>1329</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -13976,7 +13976,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
goals translations + typos fixes
</commit_message>
<xml_diff>
--- a/i18n/es.xlsx
+++ b/i18n/es.xlsx
@@ -5,16 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Other" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Parameters" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Goals" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Other" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Parameters" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A:$B</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Goals!$A$1:$F$47</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A:$B</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="ExternalData_1" vbProcedure="false">Birds!$A$1:$G$357</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ExternalData_2" vbProcedure="false">Bonuses!$A$1:$H$39</definedName>
   </definedNames>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="1443">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -4171,6 +4173,147 @@
   </si>
   <si>
     <t xml:space="preserve">[automa] Rare Species Lister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explanatory Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird in Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird in Grassland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird in Wetland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Grassland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Wetland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cavity Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bowl Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platform Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Cavity Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Bowl Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Ground Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Platform Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets of Eggs in 3 Habitats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Bird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food in Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds Cards in Hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds Worth over 4 Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds with No Eggs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds in 1 Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filled Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown Powers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White &amp; No Powers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds with Tucked Cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food Cost of Played Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invertebrate in Food Cost of Your Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fruit + Seed in Food Cost of Your Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodent + Fish in Food Cost of Your Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Goal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beak Pointing Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beak Pointing Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cubes on "Play a Bird"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds Worth Less than or Equal to 3 Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pairs of Matching Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nest Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not on Edge of Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Edge of Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokens in Any One Horizontal Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Rows with at Least One of Your Tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fewest Tokens on Bonus Spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Grassland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Wetland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Duet Tokens</t>
   </si>
   <si>
     <t xml:space="preserve">Translated</t>
@@ -4228,7 +4371,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4259,6 +4402,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -4333,19 +4483,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4379,6 +4529,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
@@ -4546,10 +4700,12 @@
   </sheetPr>
   <dimension ref="A1:K483"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E263" activeCellId="0" sqref="E263"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13381,14 +13537,16 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.71"/>
@@ -14310,10 +14468,714 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F47"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.25"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>2026</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>2027</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>2029</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>2028</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F47"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14327,55 +15189,55 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1381</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1382</v>
+        <v>1429</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1383</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1384</v>
+        <v>1431</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1385</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1386</v>
+        <v>1433</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1387</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1388</v>
+        <v>1435</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1389</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1390</v>
+        <v>1437</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1391</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1392</v>
+        <v>1439</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1393</v>
+        <v>1440</v>
       </c>
     </row>
   </sheetData>
@@ -14392,7 +15254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -14400,26 +15262,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="2" t="s">
         <v>1245</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1394</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1395</v>
+      <c r="A2" s="1" t="s">
+        <v>1442</v>
       </c>
       <c r="B2" s="10" t="b">
         <f aca="false">TRUE()</f>

</xml_diff>

<commit_message>
Translate goals and fix typos (#79)
</commit_message>
<xml_diff>
--- a/i18n/es.xlsx
+++ b/i18n/es.xlsx
@@ -5,16 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Other" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Parameters" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Goals" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Other" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Parameters" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A:$B</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Goals!$A$1:$F$47</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A:$B</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="ExternalData_1" vbProcedure="false">Birds!$A$1:$G$357</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ExternalData_2" vbProcedure="false">Bonuses!$A$1:$H$39</definedName>
   </definedNames>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="1443">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -4171,6 +4173,147 @@
   </si>
   <si>
     <t xml:space="preserve">[automa] Rare Species Lister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explanatory Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird in Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird in Grassland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird in Wetland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Grassland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Wetland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cavity Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bowl Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platform Nest Bird with Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Cavity Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Bowl Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Ground Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg in Platform Nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets of Eggs in 3 Habitats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Bird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food in Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds Cards in Hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds Worth over 4 Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds with No Eggs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds in 1 Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filled Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown Powers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White &amp; No Powers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds with Tucked Cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food Cost of Played Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invertebrate in Food Cost of Your Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fruit + Seed in Food Cost of Your Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodent + Fish in Food Cost of Your Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Goal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beak Pointing Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beak Pointing Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cubes on "Play a Bird"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds Worth Less than or Equal to 3 Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pairs of Matching Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nest Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not on Edge of Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Edge of Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokens in Any One Horizontal Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Rows with at Least One of Your Tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fewest Tokens on Bonus Spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Grassland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Wetland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Duet Tokens</t>
   </si>
   <si>
     <t xml:space="preserve">Translated</t>
@@ -4228,7 +4371,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4259,6 +4402,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -4333,19 +4483,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4379,6 +4529,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
@@ -4546,10 +4700,12 @@
   </sheetPr>
   <dimension ref="A1:K483"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E263" activeCellId="0" sqref="E263"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13381,14 +13537,16 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.71"/>
@@ -14310,10 +14468,714 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F47"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.25"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>2026</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>2027</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>2029</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>2028</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F47"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14327,55 +15189,55 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1381</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1382</v>
+        <v>1429</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1383</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1384</v>
+        <v>1431</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1385</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1386</v>
+        <v>1433</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1387</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1388</v>
+        <v>1435</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1389</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1390</v>
+        <v>1437</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1391</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1392</v>
+        <v>1439</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1393</v>
+        <v>1440</v>
       </c>
     </row>
   </sheetData>
@@ -14392,7 +15254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -14400,26 +15262,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="2" t="s">
         <v>1245</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1394</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1395</v>
+      <c r="A2" s="1" t="s">
+        <v>1442</v>
       </c>
       <c r="B2" s="10" t="b">
         <f aca="false">TRUE()</f>

</xml_diff>